<commit_message>
re-do creel stats calculations by strata and add new table
</commit_message>
<xml_diff>
--- a/data/LBN_creel-template.xlsx
+++ b/data/LBN_creel-template.xlsx
@@ -8,16 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/elh/coastland/lbn-sockeye-creel/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{085703D5-CF9E-4C43-A843-22B4AA2CF146}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C71F195-7AEA-9F4C-9D9C-D3ADB13F7BBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2160" yWindow="500" windowWidth="27620" windowHeight="16940" activeTab="2" xr2:uid="{87553B9D-CDDB-F644-AE4E-9219B22F248A}"/>
+    <workbookView xWindow="1180" yWindow="500" windowWidth="27620" windowHeight="16940" xr2:uid="{87553B9D-CDDB-F644-AE4E-9219B22F248A}"/>
   </bookViews>
   <sheets>
     <sheet name="interview recording sheet" sheetId="2" r:id="rId1"/>
     <sheet name="daily angler profile" sheetId="1" r:id="rId2"/>
     <sheet name="boat counts" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="90">
   <si>
     <t>Date</t>
   </si>
@@ -191,12 +191,6 @@
   </si>
   <si>
     <t>number of anglers in the interviewed fishing party</t>
-  </si>
-  <si>
-    <t>this group's total sk harvest / total fishing effort</t>
-  </si>
-  <si>
-    <t>this group's total sk catch / total fishing effort</t>
   </si>
   <si>
     <t>including harvests and releases</t>
@@ -372,7 +366,13 @@
   </cellStyles>
   <dxfs count="51">
     <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="general" vertical="bottom" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="90" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -390,40 +390,34 @@
       <alignment horizontal="general" vertical="bottom" textRotation="90" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="90" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="90" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="90" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="90" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="90" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="90" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="90" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <alignment horizontal="general" vertical="bottom" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="general" vertical="bottom" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="general" vertical="bottom" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="90" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="90" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="90" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="90" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="90" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="90" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="90" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="general" vertical="bottom" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -538,41 +532,45 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{CEF8FE7E-F181-AC43-8C8E-6381D5F884C6}" name="Table3" displayName="Table3" ref="A1:AB2" totalsRowShown="0" headerRowDxfId="50" dataDxfId="21">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{CEF8FE7E-F181-AC43-8C8E-6381D5F884C6}" name="Table3" displayName="Table3" ref="A1:AB2" totalsRowShown="0" headerRowDxfId="50" dataDxfId="49">
   <autoFilter ref="A1:AB2" xr:uid="{CEF8FE7E-F181-AC43-8C8E-6381D5F884C6}"/>
   <tableColumns count="28">
-    <tableColumn id="1" xr3:uid="{8820CB4F-C6B1-3F49-BC16-3363DF29C331}" name="Date" dataDxfId="49"/>
-    <tableColumn id="2" xr3:uid="{7F28E0C1-480A-9843-AD75-D3CD4BA94869}" name="Time of interview" dataDxfId="48"/>
-    <tableColumn id="3" xr3:uid="{13B275BB-3E27-D644-AB9D-97BFC117D2E8}" name="Number of anglers" dataDxfId="47"/>
-    <tableColumn id="4" xr3:uid="{6C432177-A56C-C146-A8D7-83723E264CC0}" name="Target species" dataDxfId="46"/>
-    <tableColumn id="5" xr3:uid="{15A36197-BCA9-5848-9F4B-D1E2EC096979}" name="Time angler started fishing " dataDxfId="45"/>
-    <tableColumn id="6" xr3:uid="{CEDB8C0B-B32E-DA43-883C-88A796BEC599}" name="Time angler stopped fishing" dataDxfId="44"/>
-    <tableColumn id="7" xr3:uid="{7611C2D8-4FE3-9D44-AC02-CAD55006C35F}" name="Time diff end-start" dataDxfId="43">
+    <tableColumn id="1" xr3:uid="{8820CB4F-C6B1-3F49-BC16-3363DF29C331}" name="Date" dataDxfId="48"/>
+    <tableColumn id="2" xr3:uid="{7F28E0C1-480A-9843-AD75-D3CD4BA94869}" name="Time of interview" dataDxfId="47"/>
+    <tableColumn id="3" xr3:uid="{13B275BB-3E27-D644-AB9D-97BFC117D2E8}" name="Number of anglers" dataDxfId="46"/>
+    <tableColumn id="4" xr3:uid="{6C432177-A56C-C146-A8D7-83723E264CC0}" name="Target species" dataDxfId="45"/>
+    <tableColumn id="5" xr3:uid="{15A36197-BCA9-5848-9F4B-D1E2EC096979}" name="Time angler started fishing " dataDxfId="44"/>
+    <tableColumn id="6" xr3:uid="{CEDB8C0B-B32E-DA43-883C-88A796BEC599}" name="Time angler stopped fishing" dataDxfId="43"/>
+    <tableColumn id="7" xr3:uid="{7611C2D8-4FE3-9D44-AC02-CAD55006C35F}" name="Time diff end-start" dataDxfId="42">
       <calculatedColumnFormula xml:space="preserve"> Table3[[#This Row],[Time angler stopped fishing]]-Table3[[#This Row],[Time angler started fishing ]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{A57DFE77-48C7-F644-A002-1905E8FCE3C4}" name="Total hrs fished" dataDxfId="42">
+    <tableColumn id="8" xr3:uid="{A57DFE77-48C7-F644-A002-1905E8FCE3C4}" name="Total hrs fished" dataDxfId="41">
       <calculatedColumnFormula>Table3[[#This Row],[Time diff end-start]]*24</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{BA8F9B20-AA87-9046-9382-121B8C8ACBFD}" name="Total fishing effort" dataDxfId="41"/>
-    <tableColumn id="10" xr3:uid="{A81C3DA6-6947-2643-BBC8-F657B593029D}" name="Interview location" dataDxfId="40"/>
-    <tableColumn id="11" xr3:uid="{57443B35-F1B2-FC4C-AF11-A71E00C8EE06}" name="Angler residency" dataDxfId="39"/>
-    <tableColumn id="12" xr3:uid="{C39DEC1A-742C-1548-9B14-F8C963DA8966}" name="number of days planned fishing" dataDxfId="38"/>
-    <tableColumn id="13" xr3:uid="{09F8E63D-71E6-E546-B4F7-FB190CF7D1E9}" name="SK killed" dataDxfId="37"/>
-    <tableColumn id="14" xr3:uid="{FC7939A7-1990-F14A-ABBE-509F4B035ABB}" name="RB killed " dataDxfId="36"/>
-    <tableColumn id="15" xr3:uid="{3C80862B-FDD2-1645-A16D-E6AB6A4D8B01}" name="LT killed" dataDxfId="35"/>
-    <tableColumn id="16" xr3:uid="{61F70157-6045-3D45-AA12-3DD2D624A0D5}" name="WF killed" dataDxfId="34"/>
-    <tableColumn id="17" xr3:uid="{84959A9C-9451-8840-B5C7-E9DC07FAD1CF}" name="BB killed " dataDxfId="33"/>
-    <tableColumn id="18" xr3:uid="{DA97CCEA-5C80-8E4C-88A5-18DE1DCA73FA}" name="CO killed" dataDxfId="32"/>
-    <tableColumn id="19" xr3:uid="{C1057EB1-A2FD-4547-8058-B809885A4DA0}" name="SK released" dataDxfId="31"/>
-    <tableColumn id="20" xr3:uid="{AEBE5A99-FFC8-2941-A234-B67C68D7FFEE}" name="RB released " dataDxfId="30"/>
-    <tableColumn id="21" xr3:uid="{3D7ED7F1-6861-8E42-B8A4-A4F1533CA1C9}" name="LT released" dataDxfId="29"/>
-    <tableColumn id="22" xr3:uid="{DE7B7C25-9DC4-2C4B-8713-B872277BB396}" name="WF released" dataDxfId="28"/>
-    <tableColumn id="23" xr3:uid="{31FEA4D8-817F-314F-9CEA-FD2C72F74E79}" name="BB released " dataDxfId="27"/>
-    <tableColumn id="24" xr3:uid="{96C3307E-8839-A14D-812B-B95B9CC1CD06}" name="CO released" dataDxfId="26"/>
-    <tableColumn id="25" xr3:uid="{9C3E3199-8946-2A4C-A9F2-29626C1C1E71}" name="Total sk catch" dataDxfId="25"/>
-    <tableColumn id="26" xr3:uid="{1D044555-27DD-E64B-9A92-6B7BB33FCFCA}" name="Total sk harvest" dataDxfId="24"/>
-    <tableColumn id="27" xr3:uid="{874F9EDF-A35C-6C4E-A749-3A2BE6516AEE}" name="CPUE" dataDxfId="23"/>
-    <tableColumn id="28" xr3:uid="{D26EB84F-9FAA-EA48-966B-B6C04C9ACDD3}" name="HPUE" dataDxfId="22"/>
+    <tableColumn id="9" xr3:uid="{BA8F9B20-AA87-9046-9382-121B8C8ACBFD}" name="Total fishing effort" dataDxfId="40"/>
+    <tableColumn id="10" xr3:uid="{A81C3DA6-6947-2643-BBC8-F657B593029D}" name="Interview location" dataDxfId="39"/>
+    <tableColumn id="11" xr3:uid="{57443B35-F1B2-FC4C-AF11-A71E00C8EE06}" name="Angler residency" dataDxfId="38"/>
+    <tableColumn id="12" xr3:uid="{C39DEC1A-742C-1548-9B14-F8C963DA8966}" name="number of days planned fishing" dataDxfId="37"/>
+    <tableColumn id="13" xr3:uid="{09F8E63D-71E6-E546-B4F7-FB190CF7D1E9}" name="SK killed" dataDxfId="36"/>
+    <tableColumn id="14" xr3:uid="{FC7939A7-1990-F14A-ABBE-509F4B035ABB}" name="RB killed " dataDxfId="35"/>
+    <tableColumn id="15" xr3:uid="{3C80862B-FDD2-1645-A16D-E6AB6A4D8B01}" name="LT killed" dataDxfId="34"/>
+    <tableColumn id="16" xr3:uid="{61F70157-6045-3D45-AA12-3DD2D624A0D5}" name="WF killed" dataDxfId="33"/>
+    <tableColumn id="17" xr3:uid="{84959A9C-9451-8840-B5C7-E9DC07FAD1CF}" name="BB killed " dataDxfId="32"/>
+    <tableColumn id="18" xr3:uid="{DA97CCEA-5C80-8E4C-88A5-18DE1DCA73FA}" name="CO killed" dataDxfId="31"/>
+    <tableColumn id="19" xr3:uid="{C1057EB1-A2FD-4547-8058-B809885A4DA0}" name="SK released" dataDxfId="30"/>
+    <tableColumn id="20" xr3:uid="{AEBE5A99-FFC8-2941-A234-B67C68D7FFEE}" name="RB released " dataDxfId="29"/>
+    <tableColumn id="21" xr3:uid="{3D7ED7F1-6861-8E42-B8A4-A4F1533CA1C9}" name="LT released" dataDxfId="28"/>
+    <tableColumn id="22" xr3:uid="{DE7B7C25-9DC4-2C4B-8713-B872277BB396}" name="WF released" dataDxfId="27"/>
+    <tableColumn id="23" xr3:uid="{31FEA4D8-817F-314F-9CEA-FD2C72F74E79}" name="BB released " dataDxfId="26"/>
+    <tableColumn id="24" xr3:uid="{96C3307E-8839-A14D-812B-B95B9CC1CD06}" name="CO released" dataDxfId="25"/>
+    <tableColumn id="25" xr3:uid="{9C3E3199-8946-2A4C-A9F2-29626C1C1E71}" name="Total sk catch" dataDxfId="24"/>
+    <tableColumn id="26" xr3:uid="{1D044555-27DD-E64B-9A92-6B7BB33FCFCA}" name="Total sk harvest" dataDxfId="23"/>
+    <tableColumn id="27" xr3:uid="{874F9EDF-A35C-6C4E-A749-3A2BE6516AEE}" name="CPUE" dataDxfId="22">
+      <calculatedColumnFormula>Table3[[#This Row],[Total sk catch]]/Table3[[#This Row],[Total fishing effort]]</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="28" xr3:uid="{D26EB84F-9FAA-EA48-966B-B6C04C9ACDD3}" name="HPUE" dataDxfId="21">
+      <calculatedColumnFormula>Table3[[#This Row],[Total sk harvest]]/Table3[[#This Row],[Total fishing effort]]</calculatedColumnFormula>
+    </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -601,28 +599,28 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{8A8F67EC-CF29-FC49-A2A6-8C5C0BCABAA7}" name="Table4" displayName="Table4" ref="A1:S2" totalsRowShown="0" headerRowDxfId="20" dataDxfId="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{8A8F67EC-CF29-FC49-A2A6-8C5C0BCABAA7}" name="Table4" displayName="Table4" ref="A1:S2" totalsRowShown="0" headerRowDxfId="20" dataDxfId="19">
   <autoFilter ref="A1:S2" xr:uid="{8A8F67EC-CF29-FC49-A2A6-8C5C0BCABAA7}"/>
   <tableColumns count="19">
-    <tableColumn id="1" xr3:uid="{4CF71ED7-43EA-A54E-BDC3-D8132AA312CB}" name="Date" dataDxfId="19"/>
-    <tableColumn id="19" xr3:uid="{14A57865-723A-6743-A193-D0C7ABB33C9D}" name="Day" dataDxfId="0"/>
-    <tableColumn id="2" xr3:uid="{1F3177D9-9AC1-A64B-93C4-BC4E92245F2B}" name="Weather" dataDxfId="18"/>
-    <tableColumn id="3" xr3:uid="{11DF6676-6D98-C342-AC08-DD8FDBE56C35}" name="Lake cond" dataDxfId="17"/>
-    <tableColumn id="4" xr3:uid="{17D4DAFC-AC91-1F43-A4ED-F5FD334D7497}" name="8:00" dataDxfId="16"/>
-    <tableColumn id="5" xr3:uid="{3846FE96-4C02-2746-AD1E-BF2570384E82}" name="10:00" dataDxfId="5"/>
-    <tableColumn id="6" xr3:uid="{77631E39-29A3-F048-B595-C731FA89F2E9}" name="12:00" dataDxfId="4"/>
-    <tableColumn id="7" xr3:uid="{8DF19611-41E4-AA47-81DF-E8C8CC4D255C}" name="14:00" dataDxfId="3"/>
-    <tableColumn id="8" xr3:uid="{2195B919-6FF6-F745-83D4-A681A441CC88}" name="16:00" dataDxfId="2"/>
-    <tableColumn id="9" xr3:uid="{8844AE45-8181-7346-8397-968D2823A7E5}" name="18:00" dataDxfId="1"/>
-    <tableColumn id="10" xr3:uid="{FC3012BF-603B-6A47-A9A6-CC4155F22ACF}" name="per 8:00" dataDxfId="15"/>
-    <tableColumn id="11" xr3:uid="{6177A20A-676C-B04C-8749-457E9B7CFEC5}" name="per 10:00" dataDxfId="14"/>
-    <tableColumn id="12" xr3:uid="{07017C9A-5385-CC47-9010-4CC7BF9F6E7D}" name="per 12:00" dataDxfId="13"/>
-    <tableColumn id="13" xr3:uid="{292C8769-BBE3-D84E-9F86-EF96A934DCBF}" name="per 14:00" dataDxfId="12"/>
-    <tableColumn id="14" xr3:uid="{B2F07117-D4F3-384F-981B-EB12A2B0DCA4}" name="per 16:00" dataDxfId="11"/>
-    <tableColumn id="15" xr3:uid="{B34C6A7D-C454-0241-8D0B-0FC26B91E67B}" name="per 18:00" dataDxfId="10"/>
-    <tableColumn id="16" xr3:uid="{B51F285C-CE16-EB48-AD06-0C64EDB5DF05}" name="Daily boat count" dataDxfId="9"/>
-    <tableColumn id="17" xr3:uid="{36E4DA3C-D49F-B74B-973F-EDDD312EE37D}" name="Daily boat effort" dataDxfId="8"/>
-    <tableColumn id="18" xr3:uid="{83EBAF6F-543A-5546-A0F5-1DA1306F3274}" name="Daily harvest estimate" dataDxfId="7"/>
+    <tableColumn id="1" xr3:uid="{4CF71ED7-43EA-A54E-BDC3-D8132AA312CB}" name="Date" dataDxfId="18"/>
+    <tableColumn id="19" xr3:uid="{14A57865-723A-6743-A193-D0C7ABB33C9D}" name="Day" dataDxfId="17"/>
+    <tableColumn id="2" xr3:uid="{1F3177D9-9AC1-A64B-93C4-BC4E92245F2B}" name="Weather" dataDxfId="16"/>
+    <tableColumn id="3" xr3:uid="{11DF6676-6D98-C342-AC08-DD8FDBE56C35}" name="Lake cond" dataDxfId="15"/>
+    <tableColumn id="4" xr3:uid="{17D4DAFC-AC91-1F43-A4ED-F5FD334D7497}" name="8:00" dataDxfId="14"/>
+    <tableColumn id="5" xr3:uid="{3846FE96-4C02-2746-AD1E-BF2570384E82}" name="10:00" dataDxfId="13"/>
+    <tableColumn id="6" xr3:uid="{77631E39-29A3-F048-B595-C731FA89F2E9}" name="12:00" dataDxfId="12"/>
+    <tableColumn id="7" xr3:uid="{8DF19611-41E4-AA47-81DF-E8C8CC4D255C}" name="14:00" dataDxfId="11"/>
+    <tableColumn id="8" xr3:uid="{2195B919-6FF6-F745-83D4-A681A441CC88}" name="16:00" dataDxfId="10"/>
+    <tableColumn id="9" xr3:uid="{8844AE45-8181-7346-8397-968D2823A7E5}" name="18:00" dataDxfId="9"/>
+    <tableColumn id="10" xr3:uid="{FC3012BF-603B-6A47-A9A6-CC4155F22ACF}" name="per 8:00" dataDxfId="8"/>
+    <tableColumn id="11" xr3:uid="{6177A20A-676C-B04C-8749-457E9B7CFEC5}" name="per 10:00" dataDxfId="7"/>
+    <tableColumn id="12" xr3:uid="{07017C9A-5385-CC47-9010-4CC7BF9F6E7D}" name="per 12:00" dataDxfId="6"/>
+    <tableColumn id="13" xr3:uid="{292C8769-BBE3-D84E-9F86-EF96A934DCBF}" name="per 14:00" dataDxfId="5"/>
+    <tableColumn id="14" xr3:uid="{B2F07117-D4F3-384F-981B-EB12A2B0DCA4}" name="per 16:00" dataDxfId="4"/>
+    <tableColumn id="15" xr3:uid="{B34C6A7D-C454-0241-8D0B-0FC26B91E67B}" name="per 18:00" dataDxfId="3"/>
+    <tableColumn id="16" xr3:uid="{B51F285C-CE16-EB48-AD06-0C64EDB5DF05}" name="Daily boat count" dataDxfId="2"/>
+    <tableColumn id="17" xr3:uid="{36E4DA3C-D49F-B74B-973F-EDDD312EE37D}" name="Daily boat effort" dataDxfId="1"/>
+    <tableColumn id="18" xr3:uid="{83EBAF6F-543A-5546-A0F5-1DA1306F3274}" name="Daily harvest estimate" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -947,8 +945,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B05C32D-F361-C145-B55A-ACE46C63BADF}">
   <dimension ref="A1:AB2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="V2" sqref="V2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1073,19 +1071,21 @@
         <v>48</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="Y2" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="Z2" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="AA2" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="AB2" s="1" t="s">
-        <v>51</v>
+      <c r="AA2" s="1" t="e">
+        <f>Table3[[#This Row],[Total sk catch]]/Table3[[#This Row],[Total fishing effort]]</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="AB2" s="1" t="e">
+        <f>Table3[[#This Row],[Total sk harvest]]/Table3[[#This Row],[Total fishing effort]]</f>
+        <v>#VALUE!</v>
       </c>
     </row>
   </sheetData>
@@ -1206,7 +1206,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B7F366D-7F76-FE42-A0F3-27CF65B2D71C}">
   <dimension ref="A1:S2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
@@ -1229,114 +1229,114 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="L1" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="M1" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="N1" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="O1" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="P1" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="Q1" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="E1" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="G1" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="H1" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="I1" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="J1" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="K1" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="L1" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="M1" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="N1" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="O1" s="4" t="s">
+      <c r="R1" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="S1" s="5" t="s">
         <v>66</v>
-      </c>
-      <c r="P1" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="S1" s="5" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="2" spans="1:19" ht="123" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="E2" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="G2" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="H2" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="I2" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="J2" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="I2" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="J2" s="3" t="s">
-        <v>87</v>
-      </c>
       <c r="K2" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="L2" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="M2" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="L2" s="3" t="s">
+      <c r="N2" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="M2" s="3" t="s">
+      <c r="O2" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="N2" s="3" t="s">
+      <c r="P2" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="O2" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="P2" s="3" t="s">
-        <v>81</v>
-      </c>
       <c r="Q2" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="R2" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="S2" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update template and code for processing future years creel data
</commit_message>
<xml_diff>
--- a/data/LBN_creel-template.xlsx
+++ b/data/LBN_creel-template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/elh/coastland/lbn-sockeye-creel/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C71F195-7AEA-9F4C-9D9C-D3ADB13F7BBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55340903-924A-7946-98F9-0B4B7D559604}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1180" yWindow="500" windowWidth="27620" windowHeight="16940" xr2:uid="{87553B9D-CDDB-F644-AE4E-9219B22F248A}"/>
+    <workbookView xWindow="1020" yWindow="500" windowWidth="27620" windowHeight="16940" activeTab="1" xr2:uid="{87553B9D-CDDB-F644-AE4E-9219B22F248A}"/>
   </bookViews>
   <sheets>
     <sheet name="interview recording sheet" sheetId="2" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="92">
   <si>
     <t>Date</t>
   </si>
@@ -97,15 +97,6 @@
     <t xml:space="preserve">sum of each interview's number of fishing hours </t>
   </si>
   <si>
-    <t>number of anglers in group x fishing hours</t>
-  </si>
-  <si>
-    <t>total sockeye caught</t>
-  </si>
-  <si>
-    <t>total sockeye caught and killed</t>
-  </si>
-  <si>
     <t>total sockeye caught and released</t>
   </si>
   <si>
@@ -308,16 +299,37 @@
   </si>
   <si>
     <t>Calendar date</t>
+  </si>
+  <si>
+    <t>week_day</t>
+  </si>
+  <si>
+    <t>total sockeye caught and killed that day</t>
+  </si>
+  <si>
+    <t>total sockeye caught that day</t>
+  </si>
+  <si>
+    <t>sum of (number of anglers in group x fishing hours) for that day</t>
+  </si>
+  <si>
+    <t>Area Surveyed</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -366,6 +378,12 @@
   </cellStyles>
   <dxfs count="51">
     <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <alignment horizontal="general" vertical="bottom" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -427,12 +445,6 @@
     </dxf>
     <dxf>
       <alignment horizontal="general" vertical="bottom" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -532,10 +544,11 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{CEF8FE7E-F181-AC43-8C8E-6381D5F884C6}" name="Table3" displayName="Table3" ref="A1:AB2" totalsRowShown="0" headerRowDxfId="50" dataDxfId="49">
-  <autoFilter ref="A1:AB2" xr:uid="{CEF8FE7E-F181-AC43-8C8E-6381D5F884C6}"/>
-  <tableColumns count="28">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{CEF8FE7E-F181-AC43-8C8E-6381D5F884C6}" name="Table3" displayName="Table3" ref="A1:AA2" totalsRowShown="0" headerRowDxfId="50" dataDxfId="49">
+  <autoFilter ref="A1:AA2" xr:uid="{CEF8FE7E-F181-AC43-8C8E-6381D5F884C6}"/>
+  <tableColumns count="27">
     <tableColumn id="1" xr3:uid="{8820CB4F-C6B1-3F49-BC16-3363DF29C331}" name="Date" dataDxfId="48"/>
+    <tableColumn id="27" xr3:uid="{CA3BD740-7739-6C45-A087-92B70BE1484D}" name="week_day" dataDxfId="1"/>
     <tableColumn id="2" xr3:uid="{7F28E0C1-480A-9843-AD75-D3CD4BA94869}" name="Time of interview" dataDxfId="47"/>
     <tableColumn id="3" xr3:uid="{13B275BB-3E27-D644-AB9D-97BFC117D2E8}" name="Number of anglers" dataDxfId="46"/>
     <tableColumn id="4" xr3:uid="{6C432177-A56C-C146-A8D7-83723E264CC0}" name="Target species" dataDxfId="45"/>
@@ -565,12 +578,6 @@
     <tableColumn id="24" xr3:uid="{96C3307E-8839-A14D-812B-B95B9CC1CD06}" name="CO released" dataDxfId="25"/>
     <tableColumn id="25" xr3:uid="{9C3E3199-8946-2A4C-A9F2-29626C1C1E71}" name="Total sk catch" dataDxfId="24"/>
     <tableColumn id="26" xr3:uid="{1D044555-27DD-E64B-9A92-6B7BB33FCFCA}" name="Total sk harvest" dataDxfId="23"/>
-    <tableColumn id="27" xr3:uid="{874F9EDF-A35C-6C4E-A749-3A2BE6516AEE}" name="CPUE" dataDxfId="22">
-      <calculatedColumnFormula>Table3[[#This Row],[Total sk catch]]/Table3[[#This Row],[Total fishing effort]]</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="28" xr3:uid="{D26EB84F-9FAA-EA48-966B-B6C04C9ACDD3}" name="HPUE" dataDxfId="21">
-      <calculatedColumnFormula>Table3[[#This Row],[Total sk harvest]]/Table3[[#This Row],[Total fishing effort]]</calculatedColumnFormula>
-    </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -599,28 +606,29 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{8A8F67EC-CF29-FC49-A2A6-8C5C0BCABAA7}" name="Table4" displayName="Table4" ref="A1:S2" totalsRowShown="0" headerRowDxfId="20" dataDxfId="19">
-  <autoFilter ref="A1:S2" xr:uid="{8A8F67EC-CF29-FC49-A2A6-8C5C0BCABAA7}"/>
-  <tableColumns count="19">
-    <tableColumn id="1" xr3:uid="{4CF71ED7-43EA-A54E-BDC3-D8132AA312CB}" name="Date" dataDxfId="18"/>
-    <tableColumn id="19" xr3:uid="{14A57865-723A-6743-A193-D0C7ABB33C9D}" name="Day" dataDxfId="17"/>
-    <tableColumn id="2" xr3:uid="{1F3177D9-9AC1-A64B-93C4-BC4E92245F2B}" name="Weather" dataDxfId="16"/>
-    <tableColumn id="3" xr3:uid="{11DF6676-6D98-C342-AC08-DD8FDBE56C35}" name="Lake cond" dataDxfId="15"/>
-    <tableColumn id="4" xr3:uid="{17D4DAFC-AC91-1F43-A4ED-F5FD334D7497}" name="8:00" dataDxfId="14"/>
-    <tableColumn id="5" xr3:uid="{3846FE96-4C02-2746-AD1E-BF2570384E82}" name="10:00" dataDxfId="13"/>
-    <tableColumn id="6" xr3:uid="{77631E39-29A3-F048-B595-C731FA89F2E9}" name="12:00" dataDxfId="12"/>
-    <tableColumn id="7" xr3:uid="{8DF19611-41E4-AA47-81DF-E8C8CC4D255C}" name="14:00" dataDxfId="11"/>
-    <tableColumn id="8" xr3:uid="{2195B919-6FF6-F745-83D4-A681A441CC88}" name="16:00" dataDxfId="10"/>
-    <tableColumn id="9" xr3:uid="{8844AE45-8181-7346-8397-968D2823A7E5}" name="18:00" dataDxfId="9"/>
-    <tableColumn id="10" xr3:uid="{FC3012BF-603B-6A47-A9A6-CC4155F22ACF}" name="per 8:00" dataDxfId="8"/>
-    <tableColumn id="11" xr3:uid="{6177A20A-676C-B04C-8749-457E9B7CFEC5}" name="per 10:00" dataDxfId="7"/>
-    <tableColumn id="12" xr3:uid="{07017C9A-5385-CC47-9010-4CC7BF9F6E7D}" name="per 12:00" dataDxfId="6"/>
-    <tableColumn id="13" xr3:uid="{292C8769-BBE3-D84E-9F86-EF96A934DCBF}" name="per 14:00" dataDxfId="5"/>
-    <tableColumn id="14" xr3:uid="{B2F07117-D4F3-384F-981B-EB12A2B0DCA4}" name="per 16:00" dataDxfId="4"/>
-    <tableColumn id="15" xr3:uid="{B34C6A7D-C454-0241-8D0B-0FC26B91E67B}" name="per 18:00" dataDxfId="3"/>
-    <tableColumn id="16" xr3:uid="{B51F285C-CE16-EB48-AD06-0C64EDB5DF05}" name="Daily boat count" dataDxfId="2"/>
-    <tableColumn id="17" xr3:uid="{36E4DA3C-D49F-B74B-973F-EDDD312EE37D}" name="Daily boat effort" dataDxfId="1"/>
-    <tableColumn id="18" xr3:uid="{83EBAF6F-543A-5546-A0F5-1DA1306F3274}" name="Daily harvest estimate" dataDxfId="0"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{8A8F67EC-CF29-FC49-A2A6-8C5C0BCABAA7}" name="Table4" displayName="Table4" ref="A1:T2" totalsRowShown="0" headerRowDxfId="22" dataDxfId="21">
+  <autoFilter ref="A1:T2" xr:uid="{8A8F67EC-CF29-FC49-A2A6-8C5C0BCABAA7}"/>
+  <tableColumns count="20">
+    <tableColumn id="1" xr3:uid="{4CF71ED7-43EA-A54E-BDC3-D8132AA312CB}" name="Date" dataDxfId="20"/>
+    <tableColumn id="19" xr3:uid="{14A57865-723A-6743-A193-D0C7ABB33C9D}" name="Day" dataDxfId="19"/>
+    <tableColumn id="2" xr3:uid="{1F3177D9-9AC1-A64B-93C4-BC4E92245F2B}" name="Weather" dataDxfId="18"/>
+    <tableColumn id="3" xr3:uid="{11DF6676-6D98-C342-AC08-DD8FDBE56C35}" name="Lake cond" dataDxfId="17"/>
+    <tableColumn id="4" xr3:uid="{17D4DAFC-AC91-1F43-A4ED-F5FD334D7497}" name="8:00" dataDxfId="16"/>
+    <tableColumn id="5" xr3:uid="{3846FE96-4C02-2746-AD1E-BF2570384E82}" name="10:00" dataDxfId="15"/>
+    <tableColumn id="6" xr3:uid="{77631E39-29A3-F048-B595-C731FA89F2E9}" name="12:00" dataDxfId="14"/>
+    <tableColumn id="7" xr3:uid="{8DF19611-41E4-AA47-81DF-E8C8CC4D255C}" name="14:00" dataDxfId="13"/>
+    <tableColumn id="8" xr3:uid="{2195B919-6FF6-F745-83D4-A681A441CC88}" name="16:00" dataDxfId="12"/>
+    <tableColumn id="9" xr3:uid="{8844AE45-8181-7346-8397-968D2823A7E5}" name="18:00" dataDxfId="11"/>
+    <tableColumn id="10" xr3:uid="{FC3012BF-603B-6A47-A9A6-CC4155F22ACF}" name="per 8:00" dataDxfId="10"/>
+    <tableColumn id="11" xr3:uid="{6177A20A-676C-B04C-8749-457E9B7CFEC5}" name="per 10:00" dataDxfId="9"/>
+    <tableColumn id="12" xr3:uid="{07017C9A-5385-CC47-9010-4CC7BF9F6E7D}" name="per 12:00" dataDxfId="8"/>
+    <tableColumn id="13" xr3:uid="{292C8769-BBE3-D84E-9F86-EF96A934DCBF}" name="per 14:00" dataDxfId="7"/>
+    <tableColumn id="14" xr3:uid="{B2F07117-D4F3-384F-981B-EB12A2B0DCA4}" name="per 16:00" dataDxfId="6"/>
+    <tableColumn id="15" xr3:uid="{B34C6A7D-C454-0241-8D0B-0FC26B91E67B}" name="per 18:00" dataDxfId="5"/>
+    <tableColumn id="16" xr3:uid="{B51F285C-CE16-EB48-AD06-0C64EDB5DF05}" name="Daily boat count" dataDxfId="4"/>
+    <tableColumn id="21" xr3:uid="{973A6C04-5FEB-974D-828D-0C17A2CA91AE}" name="Area Surveyed" dataDxfId="0"/>
+    <tableColumn id="17" xr3:uid="{36E4DA3C-D49F-B74B-973F-EDDD312EE37D}" name="Daily boat effort" dataDxfId="3"/>
+    <tableColumn id="18" xr3:uid="{83EBAF6F-543A-5546-A0F5-1DA1306F3274}" name="Daily harvest estimate" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -943,149 +951,136 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B05C32D-F361-C145-B55A-ACE46C63BADF}">
-  <dimension ref="A1:AB2"/>
+  <dimension ref="A1:AA2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="V2" sqref="V2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="N1" sqref="N1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="14" customWidth="1"/>
-    <col min="3" max="3" width="13.33203125" customWidth="1"/>
-    <col min="4" max="4" width="10.83203125" customWidth="1"/>
-    <col min="5" max="5" width="14.5" customWidth="1"/>
-    <col min="6" max="6" width="13.6640625" customWidth="1"/>
-    <col min="7" max="7" width="10.5" customWidth="1"/>
-    <col min="8" max="8" width="12" customWidth="1"/>
-    <col min="9" max="9" width="13" customWidth="1"/>
-    <col min="10" max="10" width="16.83203125" customWidth="1"/>
-    <col min="11" max="11" width="11.33203125" customWidth="1"/>
-    <col min="12" max="12" width="13.83203125" customWidth="1"/>
-    <col min="13" max="24" width="4.83203125" customWidth="1"/>
-    <col min="25" max="25" width="11" customWidth="1"/>
-    <col min="26" max="26" width="11.5" customWidth="1"/>
-    <col min="27" max="27" width="12.83203125" customWidth="1"/>
-    <col min="28" max="28" width="13.1640625" customWidth="1"/>
+    <col min="3" max="3" width="14" customWidth="1"/>
+    <col min="4" max="4" width="13.33203125" customWidth="1"/>
+    <col min="5" max="5" width="10.83203125" customWidth="1"/>
+    <col min="6" max="6" width="14.5" customWidth="1"/>
+    <col min="7" max="7" width="13.6640625" customWidth="1"/>
+    <col min="8" max="8" width="10.5" customWidth="1"/>
+    <col min="9" max="9" width="12" customWidth="1"/>
+    <col min="10" max="10" width="13" customWidth="1"/>
+    <col min="11" max="11" width="16.83203125" customWidth="1"/>
+    <col min="12" max="12" width="11.33203125" customWidth="1"/>
+    <col min="13" max="13" width="13.83203125" customWidth="1"/>
+    <col min="14" max="25" width="4.83203125" customWidth="1"/>
+    <col min="26" max="26" width="11" customWidth="1"/>
+    <col min="27" max="27" width="11.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" ht="67" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:27" ht="69" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="H1" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="J1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="K1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="H1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="I1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="J1" s="1" t="s">
+      <c r="N1" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="O1" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="K1" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="L1" s="1" t="s">
+      <c r="P1" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="M1" s="3" t="s">
+      <c r="Q1" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="R1" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="N1" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="O1" s="3" t="s">
+      <c r="S1" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="P1" s="3" t="s">
+      <c r="T1" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="Q1" s="3" t="s">
+      <c r="U1" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="R1" s="3" t="s">
+      <c r="V1" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="S1" s="3" t="s">
+      <c r="W1" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="T1" s="3" t="s">
+      <c r="X1" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="U1" s="3" t="s">
+      <c r="Y1" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="V1" s="3" t="s">
+      <c r="Z1" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="W1" s="3" t="s">
+      <c r="AA1" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="X1" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="Y1" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="Z1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:27" s="1" customFormat="1" ht="89" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D2" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="AA1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="AB1" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:28" s="1" customFormat="1" ht="89" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C2" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="G2" s="1">
+      <c r="H2" s="1">
         <f xml:space="preserve"> Table3[[#This Row],[Time angler stopped fishing]]-Table3[[#This Row],[Time angler started fishing ]]</f>
         <v>0</v>
       </c>
-      <c r="H2" s="1">
+      <c r="I2" s="1">
         <f>Table3[[#This Row],[Time diff end-start]]*24</f>
         <v>0</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="J2" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="Z2" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="J2" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="Y2" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="Z2" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="AA2" s="1" t="e">
-        <f>Table3[[#This Row],[Total sk catch]]/Table3[[#This Row],[Total fishing effort]]</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="AB2" s="1" t="e">
-        <f>Table3[[#This Row],[Total sk harvest]]/Table3[[#This Row],[Total fishing effort]]</f>
-        <v>#VALUE!</v>
+      <c r="AA2" s="1" t="s">
+        <v>49</v>
       </c>
     </row>
   </sheetData>
@@ -1100,7 +1095,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B05FDC82-3BB8-CF4D-A6AA-0164A2199ED0}">
   <dimension ref="A1:M2"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
       <selection activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
@@ -1176,22 +1171,22 @@
         <v>18</v>
       </c>
       <c r="F2" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="I2" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="J2" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="K2" s="1" t="s">
         <v>21</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -1204,10 +1199,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B7F366D-7F76-FE42-A0F3-27CF65B2D71C}">
-  <dimension ref="A1:S2"/>
+  <dimension ref="A1:T2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="T2" sqref="T2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1216,12 +1211,12 @@
     <col min="3" max="3" width="10.5" customWidth="1"/>
     <col min="4" max="4" width="8.6640625" customWidth="1"/>
     <col min="5" max="16" width="5.83203125" style="2" customWidth="1"/>
-    <col min="17" max="17" width="17.5" customWidth="1"/>
-    <col min="18" max="18" width="19.5" customWidth="1"/>
-    <col min="19" max="19" width="16.5" customWidth="1"/>
+    <col min="17" max="18" width="17.5" customWidth="1"/>
+    <col min="19" max="19" width="19.5" customWidth="1"/>
+    <col min="20" max="20" width="16.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" ht="53" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:20" ht="53" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1229,117 +1224,122 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="L1" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="M1" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="N1" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="O1" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="P1" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="Q1" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="R1" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="S1" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="E1" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="G1" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="H1" s="4" t="s">
+      <c r="T1" s="5" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" ht="123" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="K2" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="L2" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="M2" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="K1" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="L1" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="M1" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="N1" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="O1" s="4" t="s">
+      <c r="N2" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="O2" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="P2" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="Q2" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="R2" s="1"/>
+      <c r="S2" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="T2" s="1" t="s">
         <v>64</v>
-      </c>
-      <c r="P1" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="S1" s="5" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="2" spans="1:19" ht="123" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="I2" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="J2" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="K2" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="L2" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="M2" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="N2" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="O2" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="P2" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="Q2" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="R2" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="S2" s="1" t="s">
-        <v>67</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>

</xml_diff>